<commit_message>
modified excel trying to do pr
</commit_message>
<xml_diff>
--- a/UserStoryTask1xlsx.xlsx
+++ b/UserStoryTask1xlsx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Description:</t>
   </si>
@@ -51,6 +51,9 @@
       </rPr>
       <t xml:space="preserve"> the people seeking for skills and languages can look at what details I hold.</t>
     </r>
+  </si>
+  <si>
+    <t>Test Scenario ID</t>
   </si>
   <si>
     <t>Test Scenario</t>
@@ -1313,7 +1316,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1370,22 +1373,25 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" ht="42.75" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -1398,91 +1404,91 @@
     </row>
     <row r="7" ht="85.5" spans="1:7">
       <c r="A7" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" ht="71.25" spans="2:7">
       <c r="B8" s="10"/>
       <c r="C8" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" ht="42.75" spans="2:7">
       <c r="B9" s="10"/>
       <c r="C9" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="14"/>
       <c r="G9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" ht="57" spans="1:7">
       <c r="A10" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="57" spans="2:7">
       <c r="B11" s="10"/>
       <c r="C11" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" ht="28.5" spans="2:7">
       <c r="B12" s="10"/>
       <c r="C12" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1491,10 +1497,10 @@
     <row r="13" ht="42.75" spans="2:7">
       <c r="B13" s="10"/>
       <c r="C13" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1503,10 +1509,10 @@
     <row r="14" ht="28.5" spans="2:7">
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1515,10 +1521,10 @@
     <row r="15" ht="42.75" spans="2:7">
       <c r="B15" s="10"/>
       <c r="C15" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1527,10 +1533,10 @@
     <row r="16" ht="42.75" spans="2:7">
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1539,10 +1545,10 @@
     <row r="17" ht="42.75" spans="2:7">
       <c r="B17" s="10"/>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -1551,10 +1557,10 @@
     <row r="18" ht="42.75" spans="2:7">
       <c r="B18" s="10"/>
       <c r="C18" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1563,10 +1569,10 @@
     <row r="19" ht="42.75" spans="2:7">
       <c r="B19" s="10"/>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -1574,16 +1580,16 @@
     </row>
     <row r="20" ht="42.75" spans="1:7">
       <c r="A20" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1592,10 +1598,10 @@
     <row r="21" ht="28.5" spans="2:7">
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1604,10 +1610,10 @@
     <row r="22" ht="42.75" spans="2:7">
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1616,10 +1622,10 @@
     <row r="23" ht="28.5" spans="2:7">
       <c r="B23" s="10"/>
       <c r="C23" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1627,16 +1633,16 @@
     </row>
     <row r="24" ht="42.75" spans="1:7">
       <c r="A24" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1645,10 +1651,10 @@
     <row r="25" ht="42.75" spans="2:7">
       <c r="B25" s="4"/>
       <c r="C25" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1657,10 +1663,10 @@
     <row r="26" ht="28.5" spans="2:7">
       <c r="B26" s="4"/>
       <c r="C26" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1669,10 +1675,10 @@
     <row r="27" ht="42.75" spans="2:7">
       <c r="B27" s="4"/>
       <c r="C27" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1681,10 +1687,10 @@
     <row r="28" ht="28.5" spans="2:7">
       <c r="B28" s="4"/>
       <c r="C28" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1693,10 +1699,10 @@
     <row r="29" ht="42.75" spans="2:7">
       <c r="B29" s="4"/>
       <c r="C29" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1705,10 +1711,10 @@
     <row r="30" ht="42.75" spans="2:7">
       <c r="B30" s="4"/>
       <c r="C30" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1717,10 +1723,10 @@
     <row r="31" ht="42.75" spans="2:7">
       <c r="B31" s="4"/>
       <c r="C31" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1729,10 +1735,10 @@
     <row r="32" ht="42.75" spans="2:7">
       <c r="B32" s="4"/>
       <c r="C32" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1741,10 +1747,10 @@
     <row r="33" ht="42.75" spans="2:7">
       <c r="B33" s="4"/>
       <c r="C33" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1752,16 +1758,16 @@
     </row>
     <row r="34" ht="42.75" spans="1:7">
       <c r="A34" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1770,10 +1776,10 @@
     <row r="35" ht="28.5" spans="2:7">
       <c r="B35" s="4"/>
       <c r="C35" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1782,10 +1788,10 @@
     <row r="36" ht="42.75" spans="2:7">
       <c r="B36" s="4"/>
       <c r="C36" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1794,10 +1800,10 @@
     <row r="37" ht="28.5" spans="2:7">
       <c r="B37" s="4"/>
       <c r="C37" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>

</xml_diff>

<commit_message>
trying pr with modified excel
</commit_message>
<xml_diff>
--- a/UserStoryTask1xlsx.xlsx
+++ b/UserStoryTask1xlsx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>Description:</t>
   </si>
@@ -26,6 +26,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>As a</t>
     </r>
     <r>
@@ -40,6 +47,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>So that</t>
     </r>
     <r>
@@ -311,8 +325,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -348,38 +362,38 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,60 +416,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +455,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -484,9 +477,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,187 +515,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,6 +720,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -749,24 +772,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -784,6 +789,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -797,7 +811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -815,134 +829,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -970,12 +984,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -987,12 +995,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1315,8 +1317,8 @@
   <sheetPr/>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1383,27 +1385,27 @@
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" ht="85.5" spans="1:7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1412,45 +1414,45 @@
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" ht="71.25" spans="2:7">
-      <c r="B8" s="10"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" ht="42.75" spans="2:7">
-      <c r="B9" s="10"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="16" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" ht="57" spans="1:7">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1459,127 +1461,129 @@
       <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="16" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" ht="57" spans="2:7">
-      <c r="B11" s="10"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="16" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" ht="28.5" spans="2:7">
-      <c r="B12" s="10"/>
+    <row r="12" ht="57" spans="2:7">
+      <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="4"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" ht="42.75" spans="2:7">
-      <c r="B13" s="10"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" ht="28.5" spans="2:7">
-      <c r="B14" s="10"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" ht="42.75" spans="2:7">
-      <c r="B15" s="10"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" ht="42.75" spans="2:7">
-      <c r="B16" s="10"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" ht="42.75" spans="2:7">
-      <c r="B17" s="10"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" ht="42.75" spans="2:7">
-      <c r="B18" s="10"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" ht="42.75" spans="2:7">
-      <c r="B19" s="10"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" ht="42.75" spans="1:7">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1588,60 +1592,60 @@
       <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" ht="28.5" spans="2:7">
-      <c r="B21" s="10"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" ht="42.75" spans="2:7">
-      <c r="B22" s="10"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" ht="28.5" spans="2:7">
-      <c r="B23" s="10"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" ht="42.75" spans="1:7">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E24" s="4"/>
@@ -1653,7 +1657,7 @@
       <c r="C25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="4"/>
@@ -1665,7 +1669,7 @@
       <c r="C26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E26" s="4"/>
@@ -1677,7 +1681,7 @@
       <c r="C27" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E27" s="4"/>
@@ -1689,7 +1693,7 @@
       <c r="C28" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="4"/>
@@ -1701,7 +1705,7 @@
       <c r="C29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E29" s="4"/>
@@ -1713,7 +1717,7 @@
       <c r="C30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E30" s="4"/>
@@ -1725,7 +1729,7 @@
       <c r="C31" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E31" s="4"/>
@@ -1737,7 +1741,7 @@
       <c r="C32" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E32" s="4"/>
@@ -1749,7 +1753,7 @@
       <c r="C33" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E33" s="4"/>
@@ -1757,7 +1761,7 @@
       <c r="G33" s="4"/>
     </row>
     <row r="34" ht="42.75" spans="1:7">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1766,7 +1770,7 @@
       <c r="C34" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="7" t="s">
         <v>81</v>
       </c>
       <c r="E34" s="4"/>
@@ -1778,7 +1782,7 @@
       <c r="C35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="7" t="s">
         <v>83</v>
       </c>
       <c r="E35" s="4"/>
@@ -1790,7 +1794,7 @@
       <c r="C36" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7" t="s">
         <v>85</v>
       </c>
       <c r="E36" s="4"/>
@@ -1802,7 +1806,7 @@
       <c r="C37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E37" s="4"/>

</xml_diff>

<commit_message>
tring pr with excel trial5
</commit_message>
<xml_diff>
--- a/UserStoryTask1xlsx.xlsx
+++ b/UserStoryTask1xlsx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Description:</t>
   </si>
@@ -107,6 +107,9 @@
     <t>1.2 Check whether user can see language field after clicking on Go To Profile in USerName dropdown.</t>
   </si>
   <si>
+    <t>Follw PR1 and PR2</t>
+  </si>
+  <si>
     <t>1. Navigate to Profile page by clicking on UserName Drop down and clicking on Go To Profile.</t>
   </si>
   <si>
@@ -324,10 +327,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -362,8 +365,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -371,29 +375,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,7 +397,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -424,23 +405,23 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,6 +435,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -462,8 +450,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -471,13 +474,27 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -487,20 +504,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,43 +518,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,25 +674,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,109 +698,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,25 +713,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -748,26 +742,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -783,6 +777,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -829,130 +832,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1317,8 +1320,8 @@
   <sheetPr/>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1432,79 +1435,81 @@
         <v>17</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" ht="42.75" spans="2:7">
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="12"/>
       <c r="G9" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" ht="57" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" ht="57" spans="2:7">
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" ht="57" spans="2:7">
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" ht="42.75" spans="2:7">
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1513,10 +1518,10 @@
     <row r="14" ht="28.5" spans="2:7">
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1525,10 +1530,10 @@
     <row r="15" ht="42.75" spans="2:7">
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1537,10 +1542,10 @@
     <row r="16" ht="42.75" spans="2:7">
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1549,10 +1554,10 @@
     <row r="17" ht="42.75" spans="2:7">
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1561,10 +1566,10 @@
     <row r="18" ht="42.75" spans="2:7">
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1573,10 +1578,10 @@
     <row r="19" ht="42.75" spans="2:7">
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1584,16 +1589,16 @@
     </row>
     <row r="20" ht="42.75" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1602,10 +1607,10 @@
     <row r="21" ht="28.5" spans="2:7">
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1614,10 +1619,10 @@
     <row r="22" ht="42.75" spans="2:7">
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1626,10 +1631,10 @@
     <row r="23" ht="28.5" spans="2:7">
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1637,16 +1642,16 @@
     </row>
     <row r="24" ht="42.75" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1655,10 +1660,10 @@
     <row r="25" ht="42.75" spans="2:7">
       <c r="B25" s="4"/>
       <c r="C25" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1667,10 +1672,10 @@
     <row r="26" ht="28.5" spans="2:7">
       <c r="B26" s="4"/>
       <c r="C26" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1679,10 +1684,10 @@
     <row r="27" ht="42.75" spans="2:7">
       <c r="B27" s="4"/>
       <c r="C27" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1691,10 +1696,10 @@
     <row r="28" ht="28.5" spans="2:7">
       <c r="B28" s="4"/>
       <c r="C28" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1703,10 +1708,10 @@
     <row r="29" ht="42.75" spans="2:7">
       <c r="B29" s="4"/>
       <c r="C29" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1715,10 +1720,10 @@
     <row r="30" ht="42.75" spans="2:7">
       <c r="B30" s="4"/>
       <c r="C30" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1727,10 +1732,10 @@
     <row r="31" ht="42.75" spans="2:7">
       <c r="B31" s="4"/>
       <c r="C31" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1739,10 +1744,10 @@
     <row r="32" ht="42.75" spans="2:7">
       <c r="B32" s="4"/>
       <c r="C32" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1751,10 +1756,10 @@
     <row r="33" ht="42.75" spans="2:7">
       <c r="B33" s="4"/>
       <c r="C33" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1762,16 +1767,16 @@
     </row>
     <row r="34" ht="42.75" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1780,10 +1785,10 @@
     <row r="35" ht="28.5" spans="2:7">
       <c r="B35" s="4"/>
       <c r="C35" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1792,10 +1797,10 @@
     <row r="36" ht="42.75" spans="2:7">
       <c r="B36" s="4"/>
       <c r="C36" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1804,10 +1809,10 @@
     <row r="37" ht="28.5" spans="2:7">
       <c r="B37" s="4"/>
       <c r="C37" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>

</xml_diff>

<commit_message>
tring pr with excel2
</commit_message>
<xml_diff>
--- a/UserStoryTask1xlsx.xlsx
+++ b/UserStoryTask1xlsx.xlsx
@@ -107,7 +107,7 @@
     <t>1.2 Check whether user can see language field after clicking on Go To Profile in USerName dropdown.</t>
   </si>
   <si>
-    <t>Follw PR1 and PR2</t>
+    <t>Follow PR1 and PR2</t>
   </si>
   <si>
     <t>1. Navigate to Profile page by clicking on UserName Drop down and clicking on Go To Profile.</t>
@@ -365,24 +365,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,21 +388,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -419,24 +396,92 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,6 +489,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -451,59 +503,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,25 +518,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,12 +602,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -566,13 +632,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,121 +698,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,6 +709,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -746,22 +770,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -783,9 +792,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,23 +809,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -832,130 +832,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>